<commit_message>
Refactor audio handling and improve Excel file loading; add async loading and error handling
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,8 +456,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -476,8 +478,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -496,8 +500,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -516,8 +522,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -536,8 +544,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -556,8 +566,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -576,8 +588,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -596,8 +610,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -616,8 +632,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -636,8 +654,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -656,8 +676,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -676,8 +698,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -696,8 +720,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -716,8 +742,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -736,8 +764,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -756,8 +786,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -776,8 +808,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -796,8 +830,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -816,8 +852,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -836,8 +874,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -856,8 +896,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -876,8 +918,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -896,8 +940,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -916,8 +962,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -936,8 +984,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -956,8 +1006,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -976,8 +1028,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -996,8 +1050,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1016,8 +1072,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1036,12 +1094,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Khang</t>
+          <t>Nguyễn Thọ Khang</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1056,12 +1116,14 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>31</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Nguyễn Thọ Khang</t>
+          <t>Cù Trần Độ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1076,17 +1138,19 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>32</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cù Trần Độ</t>
+          <t>Phan Nguyễn Mai Phương</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Đông SG</t>
+          <t>RDP</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1096,12 +1160,14 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>33</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Phan Nguyễn Mai Phương</t>
+          <t>Trần Trọng Nghĩa</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1116,12 +1182,14 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>34</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Trần Trọng Nghĩa</t>
+          <t>Đinh Đức Trung</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1136,12 +1204,14 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>35</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Đinh Đức Trung</t>
+          <t>Nguyễn Nhật Quang</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1156,12 +1226,14 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>36</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nguyễn Nhật Quang</t>
+          <t>Huỳnh Hữu Trọng</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1176,12 +1248,14 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>37</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Huỳnh Hữu Trọng</t>
+          <t>Nguyễn Văn Tâm</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1196,12 +1270,14 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>38</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Tâm</t>
+          <t>Nguyễn Xuân Bảo Kỳ</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1216,12 +1292,14 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>39</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Bảo Kỳ</t>
+          <t>Phan Minh Thuần</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1236,12 +1314,14 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>40</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Phan Minh Thuần</t>
+          <t>Đái Phương Bình</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1256,12 +1336,14 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Đái Phương Bình</t>
+          <t>Trần Tuấn Phong</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1276,17 +1358,19 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Trần Tuấn Phong</t>
+          <t>Nguyễn Duy Khương</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RDP</t>
+          <t>PCN</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1296,12 +1380,14 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>43</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Nguyễn Duy Khương</t>
+          <t>Đinh Mạnh Trường</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1316,12 +1402,14 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>44</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Đinh Mạnh Trường</t>
+          <t>Huỳnh Hữu Hạng</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1336,12 +1424,14 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>45</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Huỳnh Hữu Hạng</t>
+          <t>Từ Đức Lợi</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1356,12 +1446,14 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>46</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Từ Đức Lợi</t>
+          <t xml:space="preserve">Vũ Hoàng Đức </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1376,17 +1468,19 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>47</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vũ Hoàng Đức </t>
+          <t>Nguyễn Chí Công</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PCN</t>
+          <t>TTSG</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1396,12 +1490,14 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>48</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Nguyễn Chí Công</t>
+          <t>Nguyễn Đỗ Huy Thông</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1416,12 +1512,14 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>49</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Nguyễn Đỗ Huy Thông</t>
+          <t>Lê Quang Vinh</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1436,12 +1534,14 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>50</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Lê Quang Vinh</t>
+          <t>Nguyễn Tuấn Anh</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1456,12 +1556,14 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>51</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Nguyễn Tuấn Anh</t>
+          <t>Nguyễn Xuân Vĩnh</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1476,12 +1578,14 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Vĩnh</t>
+          <t>Phan Thanh Phong</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1496,12 +1600,14 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Phan Thanh Phong</t>
+          <t>Đoàn Bảo Duy</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1516,12 +1622,14 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>54</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Đoàn Bảo Duy</t>
+          <t xml:space="preserve"> Nguyễn Hùng Tiến</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1536,12 +1644,14 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>55</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Nguyễn Hùng Tiến</t>
+          <t>Nguyễn Thanh Tú</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1556,17 +1666,19 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>56</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Tú</t>
+          <t>Nguyễn Tấn Thịnh</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>TTSG</t>
+          <t>Thủ Đức</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1576,12 +1688,14 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>58</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Nguyễn Tấn Thịnh</t>
+          <t>Hồ Viết Tình</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1596,12 +1710,14 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>59</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Hồ Viết Tình</t>
+          <t xml:space="preserve">Chế Thanh Sỉ </t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1616,12 +1732,14 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>60</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chế Thanh Sỉ </t>
+          <t>Lê Văn Thắng</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1636,12 +1754,14 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>61</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lê Văn Thắng</t>
+          <t>Phan Tuấn Kiệt</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1656,17 +1776,19 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>62</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Phan Tuấn Kiệt</t>
+          <t>Nguyễn Minh Khôi</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Thủ Đức</t>
+          <t>Bình Dương</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1676,12 +1798,14 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>63</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Trương Văn Hiếu</t>
+          <t>Nguyễn Phát Ngân</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1696,12 +1820,14 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>64</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Nguyễn Minh Khôi</t>
+          <t>Lê Chí Công</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1716,12 +1842,14 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>65</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Nguyễn Phát Ngân</t>
+          <t>Đoàn Hoài Phong</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1736,12 +1864,14 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>66</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Lê Chí Công</t>
+          <t>Trần Ngọc Thanh</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1756,12 +1886,14 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>67</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Đoàn Hoài Phong</t>
+          <t>Quan Phương Bình</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1776,12 +1908,14 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>68</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Trần Ngọc Thanh</t>
+          <t>Nguyễn Trọng Khiêm</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1796,12 +1930,14 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>69</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Quan Phương Bình</t>
+          <t>Hồ Thanh Huy</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1816,12 +1952,14 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>70</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Nguyễn Trọng Khiêm</t>
+          <t>Đỗ Trường Giang</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1836,12 +1974,14 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>71</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Hồ Thanh Huy</t>
+          <t>Trì Kim Bình</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1856,17 +1996,19 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>72</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Đỗ Trường Giang</t>
+          <t>Lê Nguyễn Hữu Toàn</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Bình Dương</t>
+          <t>Bình Phước</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1876,17 +2018,19 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>73</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Trì Kim Bình</t>
+          <t>Trần Công Ích</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Bình Dương</t>
+          <t>Đà Lạt</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1896,17 +2040,19 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>74</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Lê Nguyễn Hữu Toàn</t>
+          <t>Lê Phan Hoàng Linh</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Bình Phước</t>
+          <t>Đà Lạt</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1916,17 +2062,19 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>75</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Trần Quế Lâm</t>
+          <t>Lê Minh Hiếu</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Đà Lạt</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1936,17 +2084,19 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>76</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Trần Công Ích</t>
+          <t>Trần Thành Nguyện</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Đà Lạt</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1956,17 +2106,19 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>77</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Lê Phan Hoàng Linh</t>
+          <t>Khổng Minh Thành</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Đà Lạt</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1976,12 +2128,14 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>78</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Lê Minh Hiếu</t>
+          <t>Đỗ Nguyễn Quang Đăng Khoa</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1996,12 +2150,14 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>79</v>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Trần Thành Nguyện</t>
+          <t>Lê Quang Trí</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2016,17 +2172,19 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>80</v>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Khổng Minh Thành</t>
+          <t>Lê Văn Ngọc Tiến</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2036,37 +2194,41 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>81</v>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Đỗ Nguyễn Quang Đăng Khoa</t>
+          <t>Võ Nguyễn Thu Thủy</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>82</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Lê Quang Trí</t>
+          <t>Hồ Viết Hòa</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2076,12 +2238,14 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>83</v>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Lê Văn Ngọc Tiến</t>
+          <t>Mai Đăng Nguyên</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2096,12 +2260,14 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>84</v>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Võ Nguyễn Thu Thủy</t>
+          <t>Lê Duy Khang</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2111,284 +2277,312 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Nguyễn Đức Thiện</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Đồng Nai</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Đặng Đại Minh</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Đồng Nai</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Trịnh Minh Phát</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Đồng Nai</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Minh</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Đồng Nai</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Nguyễn Xuân Tú</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Đồng Nai</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Trần Hải Thanh</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Huỳnh Long Phương</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Thái Thành Bắc</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Lê Cao Cường</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Trần Minh Hiếu</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Bùi Thanh Hải</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Hoàng Thị Diệu Thúy</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
           <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>85</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Hồ Viết Hòa</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>86</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Mai Đăng Nguyên</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>87</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Lê Duy Khang</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>88</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Nguyễn Đức Thiện</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>89</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Đặng Đại Minh</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>90</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Trịnh Minh Phát</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>91</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Nguyễn Thanh Minh</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>92</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Nguyễn Xuân Tú</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Đồng Nai</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>93</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Trần Hải Thanh</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Lê Văn Minh</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
         <is>
           <t>Vũng Tàu</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>94</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Huỳnh Long Phương</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Lê Thiện</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
         <is>
           <t>Vũng Tàu</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>95</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Thái Thành Bắc</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>96</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Lê Cao Cường</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>97</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Trần Minh Hiếu</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>98</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Bùi Thanh Hải</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
       <c r="D98" t="inlineStr">
         <is>
           <t>DT BSS HCM</t>
@@ -2396,912 +2590,1004 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>99</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Hoàng Thị Diệu Thúy</t>
+          <t>Nguyễn Hải Đăng</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Vũng Tàu</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Lâm Trường Hải</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Phạm Quốc Toản</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Nguyễn Phượng Hoàng</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngân Đăng Hải</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Phong</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Đoàn Nhựt Phi</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Đường Lâm Khang</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Nguyễn Hải Duy</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Cần Thơ</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Lê Phú Quý</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Cà Mau</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Hậu</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Cà Mau</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Nguyễn An Thịnh</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Kiên Giang</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Phan Công Hiểu</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Kiên Giang</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Nguyễn Trúc Giang</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Kiên Giang</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Trần Trọng Nguyễn</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Sóc Trăng</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Lê Trường An</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Trà Vinh</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Thạch Vi Sal</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Trà Vinh</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Nguyễn Bảo Lộc</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Tiền Giang</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Nguyễn Thanh Hoài</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Tiền Giang</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Nguyễn Lê Bảo</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Tiền Giang</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Nguyễn Phúc Bình</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Tiền Giang</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>DT BSS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Võ Minh Phúc</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Đỗ Hoàng Minh</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Đông</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Nguyễn Thành Diêm</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Trần Đức Trường</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Cáp Ngô Minh Định</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Huỳnh Đoàn Anh Tuấn</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Thu Phương</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Nguyễn Trần Ái Thi</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Thùy Trâm</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Kinh doanh</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>DT BDS HCM</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Hải Yến</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
           <t>DT CSD HCM</t>
         </is>
       </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>100</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Lê Văn Minh</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>101</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Lê Thiện</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Vũng Tàu</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>102</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Nguyễn Hải Đăng</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>103</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Lâm Trường Hải</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>104</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Phạm Quốc Toản</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>105</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Nguyễn Phượng Hoàng</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>106</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Nguyễn Ngân Đăng Hải</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>107</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Nguyễn Thanh Phong</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>108</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Đoàn Nhựt Phi</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>109</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Đường Lâm Khang</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>110</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Nguyễn Hải Duy</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Cần Thơ</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>111</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Lê Văn Hậu</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Cà Mau</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>112</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Lê Phú Quý</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Cà Mau</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>113</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Hậu</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Cà Mau</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>114</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Nguyễn An Thịnh</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Kiên Giang</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>115</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Phan Công Hiểu</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>Kiên Giang</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>116</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Phan Triều Vĩ</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Kiên Giang</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>117</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Nguyễn Trúc Giang</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Kiên Giang</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>118</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Trần Trọng Nguyễn</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Sóc Trăng</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>119</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Lê Trường An</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>Trà Vinh</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>120</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Thạch Vi Sal</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Trà Vinh</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>121</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Nguyễn Bảo Lộc</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Tiền Giang</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>122</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>Nguyễn Thanh Hoài</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Tiền Giang</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>123</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Nguyễn Lê Bảo</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Tiền Giang</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>124</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Nguyễn Phúc Bình</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>Tiền Giang</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>DT BSS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>125</v>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Võ Minh Phúc</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>DT BDS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>126</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>Đỗ Hoàng Minh</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>DT BDS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>127</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Đông</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>DT BDS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>128</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>Nguyễn Thành Diêm</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>DT BDS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>129</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>Trần Đức Trường</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>DT BDS HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>130</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>Cáp Ngô Minh Định</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>Kinh doanh</t>
-        </is>
-      </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
-        <v>131</v>
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Huỳnh Đoàn Anh Tuấn</t>
+          <t>Lê Thị Bảo Khuyên</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
-        <v>132</v>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Thu Phương</t>
+          <t>Đỗ Chiếm Vủ</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
-        <v>133</v>
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Ái Thi</t>
+          <t>Nguyễn Thành Long</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="n">
-        <v>134</v>
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>141</t>
+        </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Thùy Trâm</t>
+          <t>Hoàng Kim Sáng</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="n">
-        <v>135</v>
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Nương</t>
+          <t>Đoàn Thị Cẩm Nhung</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="n">
-        <v>136</v>
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Đỗ Khiêm Túy Anh</t>
+          <t>Nguyễn Thị Như Quỳnh</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="n">
-        <v>137</v>
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Hải Yến</t>
+          <t>Lương Sĩ Đăng</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="n">
-        <v>138</v>
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Lê Thị Bảo Khuyên</t>
+          <t>Nguyễn Văn Hải</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="n">
-        <v>139</v>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Đỗ Chiếm Vủ</t>
+          <t>Nguyễn Trần Nguyên Khải</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="n">
-        <v>140</v>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>148</t>
+        </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Nguyễn Thành Long</t>
+          <t>Nguyễn Trần Đăng Anh</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="n">
-        <v>141</v>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Hoàng Kim Sáng</t>
+          <t>Quách Lý Duy</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="n">
-        <v>142</v>
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Đoàn Thị Cẩm Nhung</t>
+          <t>Trương Quốc Phong</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="n">
-        <v>143</v>
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Như Quỳnh</t>
+          <t>Nguyễn Văn Sơn</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="n">
-        <v>144</v>
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Lương Sĩ Đăng</t>
+          <t>Bùi Điềm Đạm</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3316,12 +3602,14 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="n">
-        <v>146</v>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Hải</t>
+          <t>Đặng Thành Luân</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3336,12 +3624,14 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="n">
-        <v>147</v>
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Nguyên Khải</t>
+          <t>Nguyễn Đắc Quốc</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3356,12 +3646,14 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="n">
-        <v>148</v>
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Đăng Anh</t>
+          <t>Đoàn Minh Quân</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3376,12 +3668,14 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="n">
-        <v>149</v>
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Quách Lý Duy</t>
+          <t>Nguyễn Trọng Huy</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3396,12 +3690,14 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="n">
-        <v>150</v>
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Trương Quốc Phong</t>
+          <t>Nguyễn Trịnh Minh Cương</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3410,146 +3706,6 @@
         </is>
       </c>
       <c r="D149" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>151</v>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Sơn</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>152</v>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>Bùi Điềm Đạm</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>153</v>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>Đặng Thành Luân</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>154</v>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>Nguyễn Đắc Quốc</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>155</v>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>Đoàn Minh Quân</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>156</v>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>Nguyễn Trọng Huy</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>157</v>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>Nguyễn Trịnh Minh Cương</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
         <is>
           <t>DT ISM HCM</t>
         </is>

</xml_diff>

<commit_message>
Update title and improve participant loading; add fade-in effect for winner announcement
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,12 +612,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nguyễn Hữu Thiện</t>
+          <t>Hoàng Trường An</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -634,12 +634,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hoàng Trường An</t>
+          <t>Đinh Trần Minh Trí</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -656,12 +656,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Đinh Trần Minh Trí</t>
+          <t>Hồ Công Hoài Bảo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,12 +678,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hồ Công Hoài Bảo</t>
+          <t>Nguyễn Lê Duy</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -700,12 +700,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nguyễn Lê Duy</t>
+          <t>Trần Chí Trung</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -722,12 +722,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Trần Chí Trung</t>
+          <t>Phan Văn Nguyên</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Phan Văn Nguyên</t>
+          <t>Đinh Văn Vinh</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -766,17 +766,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Đinh Văn Vinh</t>
+          <t>Trần Thành Nguyên</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Nam SG</t>
+          <t>Bắc SG</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,12 +788,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Trần Thành Nguyên</t>
+          <t>Trần Chánh Hùng</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -810,12 +810,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Trần Chánh Hùng</t>
+          <t>Đỗ Vũ Bình Phương</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -832,12 +832,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Đỗ Vũ Bình Phương</t>
+          <t>Nguyễn Tấn Lợi</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -854,12 +854,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Nguyễn Tấn Lợi</t>
+          <t>Nguyễn Trung Dũng</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -876,12 +876,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Nguyễn Trung Dũng</t>
+          <t>Nguyễn Trần Vủ Khang</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -898,12 +898,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Vủ Khang</t>
+          <t>Lê Văn Anh Tuấn</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -920,12 +920,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lê Văn Anh Tuấn</t>
+          <t>Nguyễn Xuân Hào</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -942,17 +942,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Hào</t>
+          <t>Lê Chí Trung</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bắc SG</t>
+          <t>Đông SG</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -964,12 +964,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lê Chí Trung</t>
+          <t>Tô Tấn Hoài</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -986,12 +986,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tô Tấn Hoài</t>
+          <t>Trần Quốc Anh</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1008,12 +1008,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Trần Quốc Anh</t>
+          <t>Nguyễn Ngọc Tiến</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1030,12 +1030,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nguyễn Ngọc Tiến</t>
+          <t>Trần Ngọc Tùng</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1052,12 +1052,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Trần Ngọc Tùng</t>
+          <t>Nguyễn Quốc Vinh</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1074,12 +1074,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Nguyễn Quốc Vinh</t>
+          <t>Nguyễn Thọ Khang</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1096,12 +1096,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Nguyễn Thọ Khang</t>
+          <t>Cù Trần Độ</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1118,17 +1118,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cù Trần Độ</t>
+          <t>Phan Nguyễn Mai Phương</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Đông SG</t>
+          <t>RDP</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1140,12 +1140,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Phan Nguyễn Mai Phương</t>
+          <t>Trần Trọng Nghĩa</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Trần Trọng Nghĩa</t>
+          <t>Nguyễn Nhật Quang</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1184,12 +1184,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Đinh Đức Trung</t>
+          <t>Huỳnh Hữu Trọng</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1206,12 +1206,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nguyễn Nhật Quang</t>
+          <t>Nguyễn Văn Tâm</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1228,12 +1228,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Huỳnh Hữu Trọng</t>
+          <t>Nguyễn Xuân Bảo Kỳ</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1250,12 +1250,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Tâm</t>
+          <t>Phan Minh Thuần</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1272,12 +1272,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Bảo Kỳ</t>
+          <t>Đái Phương Bình</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1294,12 +1294,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Phan Minh Thuần</t>
+          <t>Trần Tuấn Phong</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1316,17 +1316,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Đái Phương Bình</t>
+          <t>Nguyễn Duy Khương</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RDP</t>
+          <t>PCN</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1338,17 +1338,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Trần Tuấn Phong</t>
+          <t>Đinh Mạnh Trường</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RDP</t>
+          <t>PCN</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1360,12 +1360,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nguyễn Duy Khương</t>
+          <t>Huỳnh Hữu Hạng</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1382,12 +1382,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Đinh Mạnh Trường</t>
+          <t>Từ Đức Lợi</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1404,12 +1404,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Huỳnh Hữu Hạng</t>
+          <t xml:space="preserve">Vũ Hoàng Đức </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1426,17 +1426,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Từ Đức Lợi</t>
+          <t>Nguyễn Đỗ Huy Thông</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PCN</t>
+          <t>TTSG</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1448,17 +1448,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vũ Hoàng Đức </t>
+          <t>Lê Quang Vinh</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PCN</t>
+          <t>TTSG</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1470,12 +1470,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Nguyễn Chí Công</t>
+          <t>Nguyễn Tuấn Anh</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1492,12 +1492,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Nguyễn Đỗ Huy Thông</t>
+          <t>Nguyễn Xuân Vĩnh</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1514,12 +1514,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lê Quang Vinh</t>
+          <t>Phan Thanh Phong</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1536,12 +1536,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Nguyễn Tuấn Anh</t>
+          <t>Đoàn Bảo Duy</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1558,12 +1558,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Vĩnh</t>
+          <t xml:space="preserve"> Nguyễn Hùng Tiến</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Phan Thanh Phong</t>
+          <t>Nguyễn Thanh Tú</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1602,17 +1602,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Đoàn Bảo Duy</t>
+          <t>Nguyễn Tấn Thịnh</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>TTSG</t>
+          <t>Thủ Đức</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1624,17 +1624,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Nguyễn Hùng Tiến</t>
+          <t>Hồ Viết Tình</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>TTSG</t>
+          <t>Thủ Đức</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1646,17 +1646,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Tú</t>
+          <t xml:space="preserve">Chế Thanh Sỉ </t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>TTSG</t>
+          <t>Thủ Đức</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1668,12 +1668,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Nguyễn Tấn Thịnh</t>
+          <t>Lê Văn Thắng</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1690,12 +1690,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hồ Viết Tình</t>
+          <t>Phan Tuấn Kiệt</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1712,17 +1712,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chế Thanh Sỉ </t>
+          <t>Nguyễn Minh Khôi</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Thủ Đức</t>
+          <t>Bình Dương</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1734,17 +1734,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Lê Văn Thắng</t>
+          <t>Nguyễn Phát Ngân</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Thủ Đức</t>
+          <t>Bình Dương</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1756,17 +1756,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>66</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Phan Tuấn Kiệt</t>
+          <t>Lê Chí Công</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Thủ Đức</t>
+          <t>Bình Dương</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1778,12 +1778,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>67</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Nguyễn Minh Khôi</t>
+          <t>Đoàn Hoài Phong</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1800,12 +1800,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>68</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nguyễn Phát Ngân</t>
+          <t>Trần Ngọc Thanh</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1822,12 +1822,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>69</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Lê Chí Công</t>
+          <t>Quan Phương Bình</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1844,12 +1844,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Đoàn Hoài Phong</t>
+          <t>Nguyễn Trọng Khiêm</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1866,12 +1866,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>71</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Trần Ngọc Thanh</t>
+          <t>Hồ Thanh Huy</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1888,12 +1888,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>72</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Quan Phương Bình</t>
+          <t>Đỗ Trường Giang</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1910,12 +1910,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Nguyễn Trọng Khiêm</t>
+          <t>Trì Kim Bình</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1932,17 +1932,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>74</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Hồ Thanh Huy</t>
+          <t>Lê Nguyễn Hữu Toàn</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Bình Dương</t>
+          <t>Bình Phước</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1954,17 +1954,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>76</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Đỗ Trường Giang</t>
+          <t>Trần Công Ích</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Bình Dương</t>
+          <t>Đà Lạt</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1976,17 +1976,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>77</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Trì Kim Bình</t>
+          <t>Lê Phan Hoàng Linh</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Bình Dương</t>
+          <t>Đà Lạt</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1998,17 +1998,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Lê Nguyễn Hữu Toàn</t>
+          <t>Lê Minh Hiếu</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Bình Phước</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2020,17 +2020,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Trần Công Ích</t>
+          <t>Trần Thành Nguyện</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Đà Lạt</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2042,17 +2042,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Lê Phan Hoàng Linh</t>
+          <t>Khổng Minh Thành</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Đà Lạt</t>
+          <t>An Giang</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2064,12 +2064,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Lê Minh Hiếu</t>
+          <t>Đỗ Nguyễn Quang Đăng Khoa</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2086,12 +2086,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>82</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Trần Thành Nguyện</t>
+          <t>Lê Quang Trí</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2108,17 +2108,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>83</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Khổng Minh Thành</t>
+          <t>Lê Văn Ngọc Tiến</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2130,39 +2130,39 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>84</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Đỗ Nguyễn Quang Đăng Khoa</t>
+          <t>Võ Nguyễn Thu Thủy</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>85</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Lê Quang Trí</t>
+          <t>Hồ Viết Hòa</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>An Giang</t>
+          <t>Đồng Nai</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2174,12 +2174,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>86</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Lê Văn Ngọc Tiến</t>
+          <t>Mai Đăng Nguyên</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2196,12 +2196,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Võ Nguyễn Thu Thủy</t>
+          <t>Lê Duy Khang</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2211,19 +2211,19 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT BSS HCM</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>88</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Hồ Viết Hòa</t>
+          <t>Nguyễn Đức Thiện</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2240,12 +2240,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>90</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Mai Đăng Nguyên</t>
+          <t>Trịnh Minh Phát</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2262,12 +2262,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>91</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Lê Duy Khang</t>
+          <t>Nguyễn Thanh Minh</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2284,12 +2284,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>92</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Nguyễn Đức Thiện</t>
+          <t>Nguyễn Xuân Tú</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2306,17 +2306,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>93</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Đặng Đại Minh</t>
+          <t>Trần Hải Thanh</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Đồng Nai</t>
+          <t>Vũng Tàu</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2328,17 +2328,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>94</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Trịnh Minh Phát</t>
+          <t>Huỳnh Long Phương</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Đồng Nai</t>
+          <t>Vũng Tàu</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2350,17 +2350,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>95</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Minh</t>
+          <t>Thái Thành Bắc</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Đồng Nai</t>
+          <t>Vũng Tàu</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2372,17 +2372,17 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>96</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Nguyễn Xuân Tú</t>
+          <t>Lê Cao Cường</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Đồng Nai</t>
+          <t>Vũng Tàu</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2394,12 +2394,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>97</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Trần Hải Thanh</t>
+          <t>Trần Minh Hiếu</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>98</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Huỳnh Long Phương</t>
+          <t>Bùi Thanh Hải</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2438,12 +2438,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>99</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Thái Thành Bắc</t>
+          <t>Hoàng Thị Diệu Thúy</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2453,19 +2453,19 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>100</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Lê Cao Cường</t>
+          <t>Lê Văn Minh</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2482,12 +2482,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Trần Minh Hiếu</t>
+          <t>Lê Thiện</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2504,17 +2504,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>102</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Bùi Thanh Hải</t>
+          <t>Nguyễn Hải Đăng</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Vũng Tàu</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2526,39 +2526,39 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>103</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Hoàng Thị Diệu Thúy</t>
+          <t>Lâm Trường Hải</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Vũng Tàu</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT BSS HCM</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>104</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Lê Văn Minh</t>
+          <t>Phạm Quốc Toản</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Vũng Tàu</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2570,17 +2570,17 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>105</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Lê Thiện</t>
+          <t>Nguyễn Phượng Hoàng</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Vũng Tàu</t>
+          <t>Cần Thơ</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2592,12 +2592,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Nguyễn Hải Đăng</t>
+          <t>Nguyễn Ngân Đăng Hải</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2614,12 +2614,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>107</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Lâm Trường Hải</t>
+          <t>Nguyễn Thanh Phong</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2636,12 +2636,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Phạm Quốc Toản</t>
+          <t>Đoàn Nhựt Phi</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2658,12 +2658,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>109</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Nguyễn Phượng Hoàng</t>
+          <t>Đường Lâm Khang</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2680,12 +2680,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>110</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Nguyễn Ngân Đăng Hải</t>
+          <t>Nguyễn Hải Duy</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2702,17 +2702,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>112</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Phong</t>
+          <t>Lê Phú Quý</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Cần Thơ</t>
+          <t>Cà Mau</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2724,17 +2724,17 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>113</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Đoàn Nhựt Phi</t>
+          <t>Nguyễn Văn Hậu</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Cần Thơ</t>
+          <t>Cà Mau</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2746,17 +2746,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>114</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Đường Lâm Khang</t>
+          <t>Nguyễn An Thịnh</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Cần Thơ</t>
+          <t>Kiên Giang</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2768,17 +2768,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Nguyễn Hải Duy</t>
+          <t>Phan Công Hiểu</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Cần Thơ</t>
+          <t>Kiên Giang</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2790,17 +2790,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>117</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Lê Phú Quý</t>
+          <t>Nguyễn Trúc Giang</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Cà Mau</t>
+          <t>Kiên Giang</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2812,17 +2812,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>118</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Hậu</t>
+          <t>Trần Trọng Nguyễn</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Cà Mau</t>
+          <t>Sóc Trăng</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2834,17 +2834,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>119</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Nguyễn An Thịnh</t>
+          <t>Lê Trường An</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Kiên Giang</t>
+          <t>Trà Vinh</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2856,17 +2856,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Phan Công Hiểu</t>
+          <t>Thạch Vi Sal</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Kiên Giang</t>
+          <t>Trà Vinh</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2878,17 +2878,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>121</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Nguyễn Trúc Giang</t>
+          <t>Nguyễn Bảo Lộc</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Kiên Giang</t>
+          <t>Tiền Giang</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2900,17 +2900,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>122</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Trần Trọng Nguyễn</t>
+          <t>Nguyễn Thanh Hoài</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Sóc Trăng</t>
+          <t>Tiền Giang</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2922,17 +2922,17 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>123</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Lê Trường An</t>
+          <t>Nguyễn Lê Bảo</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Trà Vinh</t>
+          <t>Tiền Giang</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2944,17 +2944,17 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Thạch Vi Sal</t>
+          <t>Nguyễn Phúc Bình</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Trà Vinh</t>
+          <t>Tiền Giang</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2966,100 +2966,100 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Nguyễn Bảo Lộc</t>
+          <t>Võ Minh Phúc</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Tiền Giang</t>
+          <t>Kinh doanh</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT BDS HCM</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>127</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Nguyễn Thanh Hoài</t>
+          <t>Nguyễn Văn Đông</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Tiền Giang</t>
+          <t>Kinh doanh</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT BDS HCM</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Nguyễn Lê Bảo</t>
+          <t>Nguyễn Thành Diêm</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Tiền Giang</t>
+          <t>Kinh doanh</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT BDS HCM</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>129</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Nguyễn Phúc Bình</t>
+          <t>Trần Đức Trường</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Tiền Giang</t>
+          <t>Kinh doanh</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>DT BSS HCM</t>
+          <t>DT BDS HCM</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>130</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Võ Minh Phúc</t>
+          <t>Cáp Ngô Minh Định</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3076,12 +3076,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>131</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Đỗ Hoàng Minh</t>
+          <t>Huỳnh Đoàn Anh Tuấn</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3098,12 +3098,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Đông</t>
+          <t>Nguyễn Thị Thu Phương</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3120,12 +3120,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Nguyễn Thành Diêm</t>
+          <t>Nguyễn Trần Ái Thi</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3142,12 +3142,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>134</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Trần Đức Trường</t>
+          <t>Nguyễn Thị Thùy Trâm</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3164,122 +3164,122 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>137</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Cáp Ngô Minh Định</t>
+          <t>Nguyễn Thị Hải Yến</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>138</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Huỳnh Đoàn Anh Tuấn</t>
+          <t>Lê Thị Bảo Khuyên</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>140</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Thu Phương</t>
+          <t>Nguyễn Thành Long</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>141</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Ái Thi</t>
+          <t>Hoàng Kim Sáng</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT GA HCM</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>142</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Thùy Trâm</t>
+          <t>Đoàn Thị Cẩm Nhung</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Kinh doanh</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>DT BDS HCM</t>
+          <t>DT CSD HCM</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>143</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Hải Yến</t>
+          <t>Nguyễn Thị Như Quỳnh</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3296,144 +3296,144 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>144</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Lê Thị Bảo Khuyên</t>
+          <t>Lương Sĩ Đăng</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>147</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Đỗ Chiếm Vủ</t>
+          <t>Nguyễn Trần Nguyên Khải</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>148</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Nguyễn Thành Long</t>
+          <t>Nguyễn Trần Đăng Anh</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>149</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Hoàng Kim Sáng</t>
+          <t>Quách Lý Duy</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>DT GA HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>150</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Đoàn Thị Cẩm Nhung</t>
+          <t>Trương Quốc Phong</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>151</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Như Quỳnh</t>
+          <t>Nguyễn Văn Sơn</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>DT CSD HCM</t>
+          <t>DT ISM HCM</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>152</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Lương Sĩ Đăng</t>
+          <t>Bùi Điềm Đạm</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3450,12 +3450,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>153</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Hải</t>
+          <t>Đặng Thành Luân</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3472,12 +3472,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>155</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Nguyên Khải</t>
+          <t>Đoàn Minh Quân</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3494,12 +3494,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>156</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Nguyễn Trần Đăng Anh</t>
+          <t>Nguyễn Trọng Huy</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3516,12 +3516,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Quách Lý Duy</t>
+          <t>Nguyễn Trịnh Minh Cương</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3530,182 +3530,6 @@
         </is>
       </c>
       <c r="D141" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>Trương Quốc Phong</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Sơn</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>152</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>Bùi Điềm Đạm</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>153</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Đặng Thành Luân</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>154</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>Nguyễn Đắc Quốc</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>155</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>Đoàn Minh Quân</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>156</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>Nguyễn Trọng Huy</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>157</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>Nguyễn Trịnh Minh Cương</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>DT ISM HCM</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
         <is>
           <t>DT ISM HCM</t>
         </is>

</xml_diff>